<commit_message>
Wins and Looses are now tracked
</commit_message>
<xml_diff>
--- a/userSystem/leaderboard.xlsx
+++ b/userSystem/leaderboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\LeaderBoard\avengers-leaderboard\userSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8AF8981-A150-4C63-9719-2EE503C32F3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1D75F5-151F-430F-823C-E85067D76B70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5835" yWindow="9540" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>User</t>
   </si>
@@ -47,20 +47,32 @@
   </si>
   <si>
     <t>giggo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wins </t>
+  </si>
+  <si>
+    <t>Looses</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -72,8 +84,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF8E98A5"/>
+        <fgColor theme="3"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -89,9 +107,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -396,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,7 +428,7 @@
     <col min="9" max="9" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -419,8 +438,14 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -430,8 +455,14 @@
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -441,8 +472,14 @@
       <c r="C3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -452,8 +489,14 @@
       <c r="C4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -463,8 +506,14 @@
       <c r="C5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -474,8 +523,14 @@
       <c r="C6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -483,6 +538,12 @@
         <v>1013</v>
       </c>
       <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
         <v>0</v>
       </c>
     </row>

</xml_diff>